<commit_message>
liste des structures a hu forecees
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/sein DIBH.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/sein DIBH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
     <t>Ring_PTVboost</t>
   </si>
   <si>
-    <t>Body RL</t>
+    <t>Body_RL</t>
   </si>
 </sst>
 </file>
@@ -2235,8 +2235,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,7 +2463,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>